<commit_message>
updated documents, removed unused and not practical chart generating class
</commit_message>
<xml_diff>
--- a/documents/xlsxdoc.xlsx
+++ b/documents/xlsxdoc.xlsx
@@ -12,25 +12,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Kacper</t>
   </si>
   <si>
     <t>Transaction Dates: 
-07/03/2024—10/15/2024</t>
+06/23/2024—10/15/2024</t>
   </si>
   <si>
     <t>Report Generated on:
-09/02/2024 13:13:54</t>
+09/02/2024 13:53:40</t>
   </si>
   <si>
     <t>Balance:
-1830.00</t>
+1679.01</t>
   </si>
   <si>
     <t>Total Expenses:
-7370.00</t>
+7520.99</t>
   </si>
   <si>
     <t>Total Income:
@@ -115,6 +115,9 @@
     <t>2024-08-24</t>
   </si>
   <si>
+    <t>Salary</t>
+  </si>
+  <si>
     <t>5200.00</t>
   </si>
   <si>
@@ -143,6 +146,18 @@
   </si>
   <si>
     <t>Went to Turkey for the summer holydays.</t>
+  </si>
+  <si>
+    <t>2024-06-23</t>
+  </si>
+  <si>
+    <t>House and Garden</t>
+  </si>
+  <si>
+    <t>150.99</t>
+  </si>
+  <si>
+    <t>Garden hose and watering can for my garden</t>
   </si>
 </sst>
 </file>
@@ -233,7 +248,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -386,47 +401,64 @@
         <v>21</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>